<commit_message>
Finalization of PAD results for AGU
Finalization of PAD results for AGU
</commit_message>
<xml_diff>
--- a/Sensitivity of photoelectron corrections.xlsx
+++ b/Sensitivity of photoelectron corrections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="9495" windowHeight="15090"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="9495" windowHeight="15090" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Inferred Counts" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="4">
   <si>
     <t>n photo</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>Erg</t>
+  </si>
+  <si>
+    <t>error bar</t>
   </si>
 </sst>
 </file>
@@ -1460,7 +1463,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>jN!$G$38:$G$47</c:f>
+              <c:f>jN!$C$51:$C$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1934,7 +1937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
@@ -3002,8 +3005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3996,10 +3999,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N51" sqref="N51:N60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4577,13 +4580,6 @@
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="4"/>
@@ -4593,16 +4589,6 @@
         <v>0</v>
       </c>
       <c r="D38" s="2"/>
-      <c r="E38" s="1">
-        <v>109053700.59</v>
-      </c>
-      <c r="F38" s="6">
-        <v>107712223.022</v>
-      </c>
-      <c r="G38" s="2">
-        <f>E38-F38</f>
-        <v>1341477.5680000037</v>
-      </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="4"/>
@@ -4612,16 +4598,6 @@
         <v>0</v>
       </c>
       <c r="D39" s="2"/>
-      <c r="E39" s="1">
-        <v>99762802.872199997</v>
-      </c>
-      <c r="F39" s="6">
-        <v>98334401.632599995</v>
-      </c>
-      <c r="G39" s="2">
-        <f t="shared" ref="G39:G47" si="7">E39-F39</f>
-        <v>1428401.2396000028</v>
-      </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="4"/>
@@ -4631,16 +4607,6 @@
         <v>0</v>
       </c>
       <c r="D40" s="2"/>
-      <c r="E40" s="1">
-        <v>85584514.363299996</v>
-      </c>
-      <c r="F40" s="6">
-        <v>85680245.817699999</v>
-      </c>
-      <c r="G40" s="2">
-        <f t="shared" si="7"/>
-        <v>-95731.454400002956</v>
-      </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="4"/>
@@ -4650,16 +4616,6 @@
         <v>0</v>
       </c>
       <c r="D41" s="2"/>
-      <c r="E41" s="1">
-        <v>61454150.6589</v>
-      </c>
-      <c r="F41" s="6">
-        <v>63499455.562299997</v>
-      </c>
-      <c r="G41" s="2">
-        <f t="shared" si="7"/>
-        <v>-2045304.9033999965</v>
-      </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="4"/>
@@ -4669,16 +4625,6 @@
         <v>0</v>
       </c>
       <c r="D42" s="2"/>
-      <c r="E42" s="1">
-        <v>35656993.198799998</v>
-      </c>
-      <c r="F42" s="6">
-        <v>35043716.854699999</v>
-      </c>
-      <c r="G42" s="2">
-        <f t="shared" si="7"/>
-        <v>613276.34409999847</v>
-      </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="4"/>
@@ -4688,16 +4634,6 @@
         <v>0</v>
       </c>
       <c r="D43" s="2"/>
-      <c r="E43" s="1">
-        <v>19838951.280999999</v>
-      </c>
-      <c r="F43" s="6">
-        <v>20538227.4027</v>
-      </c>
-      <c r="G43" s="2">
-        <f t="shared" si="7"/>
-        <v>-699276.12170000002</v>
-      </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="4"/>
@@ -4707,16 +4643,6 @@
         <v>0</v>
       </c>
       <c r="D44" s="2"/>
-      <c r="E44" s="1">
-        <v>10354627.713400001</v>
-      </c>
-      <c r="F44" s="6">
-        <v>10560048.6954</v>
-      </c>
-      <c r="G44" s="2">
-        <f t="shared" si="7"/>
-        <v>-205420.98199999891</v>
-      </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="4"/>
@@ -4726,16 +4652,6 @@
         <v>0</v>
       </c>
       <c r="D45" s="2"/>
-      <c r="E45" s="1">
-        <v>4493881.3726599999</v>
-      </c>
-      <c r="F45" s="6">
-        <v>4093395.0691800001</v>
-      </c>
-      <c r="G45" s="2">
-        <f t="shared" si="7"/>
-        <v>400486.30347999977</v>
-      </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="4"/>
@@ -4745,16 +4661,6 @@
         <v>0</v>
       </c>
       <c r="D46" s="2"/>
-      <c r="E46" s="1">
-        <v>1710851.51722</v>
-      </c>
-      <c r="F46" s="6">
-        <v>1622259.6176</v>
-      </c>
-      <c r="G46" s="2">
-        <f t="shared" si="7"/>
-        <v>88591.89962000004</v>
-      </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="4"/>
@@ -4764,18 +4670,15 @@
         <v>0</v>
       </c>
       <c r="D47" s="2"/>
-      <c r="E47" s="1">
-        <v>1485803.0416999999</v>
-      </c>
-      <c r="F47" s="6">
-        <v>1492517.5363</v>
-      </c>
-      <c r="G47" s="2">
-        <f t="shared" si="7"/>
-        <v>-6714.4946000000928</v>
-      </c>
-    </row>
-    <row r="50" spans="5:12">
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="C50" s="2"/>
       <c r="E50" s="4" t="s">
         <v>1</v>
       </c>
@@ -4790,8 +4693,21 @@
         <v>0.8</v>
       </c>
       <c r="L50" s="2"/>
-    </row>
-    <row r="51" spans="5:12">
+      <c r="N50" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" s="1">
+        <v>109053700.59</v>
+      </c>
+      <c r="B51" s="6">
+        <v>107712223.022</v>
+      </c>
+      <c r="C51" s="2">
+        <f>A51-B51</f>
+        <v>1341477.5680000037</v>
+      </c>
       <c r="E51" s="1">
         <v>108008960.06900001</v>
       </c>
@@ -4812,8 +4728,22 @@
         <f>J51-K51</f>
         <v>5667445.023999989</v>
       </c>
-    </row>
-    <row r="52" spans="5:12">
+      <c r="N51" s="3">
+        <f>ABS(L51-C51)/2</f>
+        <v>2162983.7279999927</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" s="1">
+        <v>99762802.872199997</v>
+      </c>
+      <c r="B52" s="6">
+        <v>98334401.632599995</v>
+      </c>
+      <c r="C52" s="2">
+        <f t="shared" ref="C52:C60" si="7">A52-B52</f>
+        <v>1428401.2396000028</v>
+      </c>
       <c r="E52" s="1">
         <v>99203153.916099995</v>
       </c>
@@ -4834,8 +4764,22 @@
         <f t="shared" ref="L52:L60" si="9">J52-K52</f>
         <v>3746237.7827000022</v>
       </c>
-    </row>
-    <row r="53" spans="5:12">
+      <c r="N52" s="3">
+        <f t="shared" ref="N52:N60" si="10">ABS(L52-C52)/2</f>
+        <v>1158918.2715499997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" s="1">
+        <v>85584514.363299996</v>
+      </c>
+      <c r="B53" s="6">
+        <v>85680245.817699999</v>
+      </c>
+      <c r="C53" s="2">
+        <f t="shared" si="7"/>
+        <v>-95731.454400002956</v>
+      </c>
       <c r="E53" s="1">
         <v>85284684.022400007</v>
       </c>
@@ -4856,8 +4800,22 @@
         <f t="shared" si="9"/>
         <v>1146381.9271000028</v>
       </c>
-    </row>
-    <row r="54" spans="5:12">
+      <c r="N53" s="3">
+        <f t="shared" si="10"/>
+        <v>621056.69075000286</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="1">
+        <v>61454150.6589</v>
+      </c>
+      <c r="B54" s="6">
+        <v>63499455.562299997</v>
+      </c>
+      <c r="C54" s="2">
+        <f t="shared" si="7"/>
+        <v>-2045304.9033999965</v>
+      </c>
       <c r="E54" s="1">
         <v>61293450.238700002</v>
       </c>
@@ -4878,8 +4836,22 @@
         <f t="shared" si="9"/>
         <v>-1379353.0420999974</v>
       </c>
-    </row>
-    <row r="55" spans="5:12">
+      <c r="N54" s="3">
+        <f t="shared" si="10"/>
+        <v>332975.93064999953</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="1">
+        <v>35656993.198799998</v>
+      </c>
+      <c r="B55" s="6">
+        <v>35043716.854699999</v>
+      </c>
+      <c r="C55" s="2">
+        <f t="shared" si="7"/>
+        <v>613276.34409999847</v>
+      </c>
       <c r="E55" s="1">
         <v>35570838.539300002</v>
       </c>
@@ -4900,8 +4872,22 @@
         <f t="shared" si="9"/>
         <v>970446.13920000196</v>
       </c>
-    </row>
-    <row r="56" spans="5:12">
+      <c r="N55" s="3">
+        <f t="shared" si="10"/>
+        <v>178584.89755000174</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" s="1">
+        <v>19838951.280999999</v>
+      </c>
+      <c r="B56" s="6">
+        <v>20538227.4027</v>
+      </c>
+      <c r="C56" s="2">
+        <f t="shared" si="7"/>
+        <v>-699276.12170000002</v>
+      </c>
       <c r="E56" s="1">
         <v>19792738.2612</v>
       </c>
@@ -4922,8 +4908,22 @@
         <f t="shared" si="9"/>
         <v>-507603.61230000108</v>
       </c>
-    </row>
-    <row r="57" spans="5:12">
+      <c r="N56" s="3">
+        <f t="shared" si="10"/>
+        <v>95836.254699999467</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="1">
+        <v>10354627.713400001</v>
+      </c>
+      <c r="B57" s="6">
+        <v>10560048.6954</v>
+      </c>
+      <c r="C57" s="2">
+        <f t="shared" si="7"/>
+        <v>-205420.98199999891</v>
+      </c>
       <c r="E57" s="1">
         <v>10329820.3729</v>
       </c>
@@ -4944,8 +4944,22 @@
         <f t="shared" si="9"/>
         <v>-102474.86979999952</v>
       </c>
-    </row>
-    <row r="58" spans="5:12">
+      <c r="N57" s="3">
+        <f t="shared" si="10"/>
+        <v>51473.056099999696</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" s="1">
+        <v>4493881.3726599999</v>
+      </c>
+      <c r="B58" s="6">
+        <v>4093395.0691800001</v>
+      </c>
+      <c r="C58" s="2">
+        <f t="shared" si="7"/>
+        <v>400486.30347999977</v>
+      </c>
       <c r="E58" s="1">
         <v>4480550.1858599996</v>
       </c>
@@ -4966,8 +4980,22 @@
         <f t="shared" si="9"/>
         <v>455842.11754000047</v>
       </c>
-    </row>
-    <row r="59" spans="5:12">
+      <c r="N58" s="3">
+        <f t="shared" si="10"/>
+        <v>27677.907030000351</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" s="1">
+        <v>1710851.51722</v>
+      </c>
+      <c r="B59" s="6">
+        <v>1622259.6176</v>
+      </c>
+      <c r="C59" s="2">
+        <f t="shared" si="7"/>
+        <v>88591.89962000004</v>
+      </c>
       <c r="E59" s="1">
         <v>1703682.03262</v>
       </c>
@@ -4988,8 +5016,22 @@
         <f t="shared" si="9"/>
         <v>118381.82196999993</v>
       </c>
-    </row>
-    <row r="60" spans="5:12">
+      <c r="N59" s="3">
+        <f t="shared" si="10"/>
+        <v>14894.961174999946</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="1">
+        <v>1485803.0416999999</v>
+      </c>
+      <c r="B60" s="6">
+        <v>1492517.5363</v>
+      </c>
+      <c r="C60" s="2">
+        <f t="shared" si="7"/>
+        <v>-6714.4946000000928</v>
+      </c>
       <c r="E60" s="1">
         <v>1481942.05642</v>
       </c>
@@ -5009,6 +5051,10 @@
       <c r="L60" s="2">
         <f t="shared" si="9"/>
         <v>9339.5480899999384</v>
+      </c>
+      <c r="N60" s="3">
+        <f t="shared" si="10"/>
+        <v>8027.0213450000156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>